<commit_message>
add the data set and fix a double counting issue in system_performance symmary file
</commit_message>
<xml_diff>
--- a/dataset_v1/Usecases_FOCUSING_Framework/FOCUSING_Use_cases_master_file_v1.xlsx
+++ b/dataset_v1/Usecases_FOCUSING_Framework/FOCUSING_Use_cases_master_file_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18016\Documents\GitHub\DTALite\dataset_v1\Usecases_FOCUSING_Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98BAAAA-A4E2-4683-BFE0-6367DB6A4932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520AA2FA-2E68-4BE9-B311-7DD0063FCD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{52FDBE42-1421-4610-A79E-F608848648A7}"/>
   </bookViews>
@@ -729,7 +729,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
test of real time information user class
we enable the two-corridor test cases with 4 departure time periods and 2 user class groups.
</commit_message>
<xml_diff>
--- a/dataset_v1/Usecases_FOCUSING_Framework/FOCUSING_Use_cases_master_file_v1.xlsx
+++ b/dataset_v1/Usecases_FOCUSING_Framework/FOCUSING_Use_cases_master_file_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18016\Documents\GitHub\DTALite\dataset_v1\Usecases_FOCUSING_Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520AA2FA-2E68-4BE9-B311-7DD0063FCD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BCE862-DA85-43C0-AF9C-6BC62F1405BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{52FDBE42-1421-4610-A79E-F608848648A7}"/>
   </bookViews>
@@ -729,7 +729,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D24" sqref="D24:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>